<commit_message>
Adding code to test database queries
</commit_message>
<xml_diff>
--- a/Automation/DataFiles/employees.xlsx
+++ b/Automation/DataFiles/employees.xlsx
@@ -55,12 +55,22 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -110,7 +121,7 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>A2&gt;101</f>
       </c>
     </row>
@@ -124,7 +135,7 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>A3&gt;101</f>
       </c>
     </row>
@@ -138,7 +149,7 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f>A4&gt;101</f>
       </c>
     </row>

</xml_diff>